<commit_message>
python 3 version support
</commit_message>
<xml_diff>
--- a/Output Data/Crpo/Common_folder/API_Performance_Chart_Report.xlsx
+++ b/Output Data/Crpo/Common_folder/API_Performance_Chart_Report.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Dashboard" sheetId="1" state="visible" r:id="rId2"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1371" uniqueCount="331">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1475" uniqueCount="356">
   <si>
     <t xml:space="preserve">get_tenant_details</t>
   </si>
@@ -656,6 +656,54 @@
     <t xml:space="preserve">05:11:PM</t>
   </si>
   <si>
+    <t xml:space="preserve">05:13:PM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2021-04-22</t>
+  </si>
+  <si>
+    <t xml:space="preserve">01:59:PM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">02:17:PM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">02:18:PM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2021-04-23</t>
+  </si>
+  <si>
+    <t xml:space="preserve">08:10:AM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">08:12:AM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">08:13:AM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">05:15:PM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">05:17:PM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">05:19:PM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2021-04-26</t>
+  </si>
+  <si>
+    <t xml:space="preserve">11:55:AM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">11:56:AM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">11:58:AM</t>
+  </si>
+  <si>
     <t xml:space="preserve">07:41:PM</t>
   </si>
   <si>
@@ -782,6 +830,24 @@
     <t xml:space="preserve">05:09:PM</t>
   </si>
   <si>
+    <t xml:space="preserve">08:18:AM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">05:18:PM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">05:22:PM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">05:25:PM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">05:30:PM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">12:00:PM</t>
+  </si>
+  <si>
     <t xml:space="preserve">07:43:PM</t>
   </si>
   <si>
@@ -800,9 +866,6 @@
     <t xml:space="preserve">11:24:AM</t>
   </si>
   <si>
-    <t xml:space="preserve">08:10:AM</t>
-  </si>
-  <si>
     <t xml:space="preserve">08:21:AM</t>
   </si>
   <si>
@@ -932,6 +995,12 @@
     <t xml:space="preserve">05:10:PM</t>
   </si>
   <si>
+    <t xml:space="preserve">08:11:AM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">05:16:PM</t>
+  </si>
+  <si>
     <t xml:space="preserve">07:44:PM</t>
   </si>
   <si>
@@ -941,9 +1010,6 @@
     <t xml:space="preserve">08:16:AM</t>
   </si>
   <si>
-    <t xml:space="preserve">08:18:AM</t>
-  </si>
-  <si>
     <t xml:space="preserve">04:29:PM</t>
   </si>
   <si>
@@ -1017,6 +1083,15 @@
   </si>
   <si>
     <t xml:space="preserve">05:12:PM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">02:02:PM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">05:24:PM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">11:59:AM</t>
   </si>
 </sst>
 </file>
@@ -1160,31 +1235,31 @@
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1331,16 +1406,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>1.07428282891566</c:v>
+                  <c:v>1.02920023687151</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.41015870658683</c:v>
+                  <c:v>2.38901973259668</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.949352507784431</c:v>
+                  <c:v>0.915364274860335</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3.81975222035928</c:v>
+                  <c:v>3.81263425111111</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1407,16 +1482,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>0.884868979518072</c:v>
+                  <c:v>0.853480106145252</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.1477044742515</c:v>
+                  <c:v>2.28727468066298</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.1881117497006</c:v>
+                  <c:v>1.14078570167598</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2.02643083473054</c:v>
+                  <c:v>1.99645761222222</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1483,16 +1558,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>0.914744578313253</c:v>
+                  <c:v>0.877927574301676</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.57857243113773</c:v>
+                  <c:v>1.75045849060774</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.22129534850299</c:v>
+                  <c:v>1.17334780782123</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.89275095329341</c:v>
+                  <c:v>1.84160820777778</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1559,16 +1634,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>1.54995921445783</c:v>
+                  <c:v>1.52986577988827</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.28203454491018</c:v>
+                  <c:v>2.45745003756906</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.80089136886228</c:v>
+                  <c:v>1.76383223463687</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2.74385565988024</c:v>
+                  <c:v>2.71625712777778</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1635,16 +1710,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>0.841958362650603</c:v>
+                  <c:v>0.817053955307263</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.57990958083832</c:v>
+                  <c:v>1.68919568839779</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.10696194610779</c:v>
+                  <c:v>1.06898891396648</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.63361053652695</c:v>
+                  <c:v>1.59409121444444</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1652,11 +1727,11 @@
         </c:ser>
         <c:gapWidth val="150"/>
         <c:overlap val="-10"/>
-        <c:axId val="59723609"/>
-        <c:axId val="76039697"/>
+        <c:axId val="25917763"/>
+        <c:axId val="70168716"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="59723609"/>
+        <c:axId val="25917763"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1722,14 +1797,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="76039697"/>
+        <c:crossAx val="70168716"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="76039697"/>
+        <c:axId val="70168716"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1795,7 +1870,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="59723609"/>
+        <c:crossAx val="25917763"/>
         <c:crosses val="autoZero"/>
       </c:valAx>
       <c:spPr>
@@ -1887,7 +1962,7 @@
   </sheetPr>
   <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A2" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B24" activeCellId="0" sqref="B24"/>
     </sheetView>
   </sheetViews>
@@ -1924,19 +1999,19 @@
         <v>5</v>
       </c>
       <c r="B2" s="1" t="n">
-        <v>1.07428282891566</v>
+        <v>1.02920023687151</v>
       </c>
       <c r="C2" s="1" t="n">
-        <v>0.884868979518072</v>
+        <v>0.853480106145252</v>
       </c>
       <c r="D2" s="1" t="n">
-        <v>0.914744578313253</v>
+        <v>0.877927574301676</v>
       </c>
       <c r="E2" s="1" t="n">
-        <v>1.54995921445783</v>
+        <v>1.52986577988827</v>
       </c>
       <c r="F2" s="1" t="n">
-        <v>0.841958362650603</v>
+        <v>0.817053955307263</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1944,19 +2019,19 @@
         <v>6</v>
       </c>
       <c r="B3" s="1" t="n">
-        <v>2.41015870658683</v>
+        <v>2.38901973259668</v>
       </c>
       <c r="C3" s="1" t="n">
-        <v>2.1477044742515</v>
+        <v>2.28727468066298</v>
       </c>
       <c r="D3" s="1" t="n">
-        <v>1.57857243113773</v>
+        <v>1.75045849060774</v>
       </c>
       <c r="E3" s="1" t="n">
-        <v>2.28203454491018</v>
+        <v>2.45745003756906</v>
       </c>
       <c r="F3" s="1" t="n">
-        <v>1.57990958083832</v>
+        <v>1.68919568839779</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1964,19 +2039,19 @@
         <v>7</v>
       </c>
       <c r="B4" s="1" t="n">
-        <v>0.949352507784431</v>
+        <v>0.915364274860335</v>
       </c>
       <c r="C4" s="1" t="n">
-        <v>1.1881117497006</v>
+        <v>1.14078570167598</v>
       </c>
       <c r="D4" s="1" t="n">
-        <v>1.22129534850299</v>
+        <v>1.17334780782123</v>
       </c>
       <c r="E4" s="1" t="n">
-        <v>1.80089136886228</v>
+        <v>1.76383223463687</v>
       </c>
       <c r="F4" s="1" t="n">
-        <v>1.10696194610779</v>
+        <v>1.06898891396648</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1984,19 +2059,19 @@
         <v>8</v>
       </c>
       <c r="B5" s="1" t="n">
-        <v>3.81975222035928</v>
+        <v>3.81263425111111</v>
       </c>
       <c r="C5" s="1" t="n">
-        <v>2.02643083473054</v>
+        <v>1.99645761222222</v>
       </c>
       <c r="D5" s="1" t="n">
-        <v>1.89275095329341</v>
+        <v>1.84160820777778</v>
       </c>
       <c r="E5" s="1" t="n">
-        <v>2.74385565988024</v>
+        <v>2.71625712777778</v>
       </c>
       <c r="F5" s="1" t="n">
-        <v>1.63361053652695</v>
+        <v>1.59409121444444</v>
       </c>
     </row>
   </sheetData>
@@ -2018,8 +2093,8 @@
   </sheetPr>
   <dimension ref="A1:I1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A152" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C160" activeCellId="0" sqref="C160"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A170" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A180" activeCellId="0" sqref="A180"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5776,7 +5851,7 @@
       <c r="H161" s="4"/>
       <c r="I161" s="4"/>
     </row>
-    <row r="162" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="162" customFormat="false" ht="23.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A162" s="4" t="s">
         <v>200</v>
       </c>
@@ -5801,7 +5876,7 @@
       <c r="H162" s="4"/>
       <c r="I162" s="4"/>
     </row>
-    <row r="163" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="163" customFormat="false" ht="23.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A163" s="4" t="s">
         <v>203</v>
       </c>
@@ -5826,7 +5901,7 @@
       <c r="H163" s="4"/>
       <c r="I163" s="4"/>
     </row>
-    <row r="164" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="164" customFormat="false" ht="23.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A164" s="4" t="s">
         <v>203</v>
       </c>
@@ -5851,7 +5926,7 @@
       <c r="H164" s="4"/>
       <c r="I164" s="4"/>
     </row>
-    <row r="165" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="165" customFormat="false" ht="23.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A165" s="4" t="s">
         <v>203</v>
       </c>
@@ -5876,7 +5951,7 @@
       <c r="H165" s="4"/>
       <c r="I165" s="4"/>
     </row>
-    <row r="166" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="166" customFormat="false" ht="23.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A166" s="4" t="s">
         <v>207</v>
       </c>
@@ -5901,7 +5976,7 @@
       <c r="H166" s="4"/>
       <c r="I166" s="4"/>
     </row>
-    <row r="167" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="167" customFormat="false" ht="23.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A167" s="4" t="s">
         <v>207</v>
       </c>
@@ -5925,6 +6000,331 @@
       </c>
       <c r="H167" s="4"/>
       <c r="I167" s="4"/>
+    </row>
+    <row r="168" customFormat="false" ht="23.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A168" s="4" t="s">
+        <v>207</v>
+      </c>
+      <c r="B168" s="4" t="s">
+        <v>210</v>
+      </c>
+      <c r="C168" s="4" t="n">
+        <v>0.343108</v>
+      </c>
+      <c r="D168" s="4" t="n">
+        <v>0.8795912</v>
+      </c>
+      <c r="E168" s="4" t="n">
+        <v>0.2981296</v>
+      </c>
+      <c r="F168" s="4" t="n">
+        <v>1.130887</v>
+      </c>
+      <c r="G168" s="4" t="n">
+        <v>0.3344664</v>
+      </c>
+      <c r="H168" s="4"/>
+      <c r="I168" s="4"/>
+    </row>
+    <row r="169" customFormat="false" ht="23.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A169" s="4" t="s">
+        <v>211</v>
+      </c>
+      <c r="B169" s="4" t="s">
+        <v>212</v>
+      </c>
+      <c r="C169" s="4" t="n">
+        <v>0.3818272</v>
+      </c>
+      <c r="D169" s="4" t="n">
+        <v>0.3426448</v>
+      </c>
+      <c r="E169" s="4" t="n">
+        <v>0.3409916</v>
+      </c>
+      <c r="F169" s="4" t="n">
+        <v>1.1209198</v>
+      </c>
+      <c r="G169" s="4" t="n">
+        <v>0.3829526</v>
+      </c>
+      <c r="H169" s="4"/>
+      <c r="I169" s="4"/>
+    </row>
+    <row r="170" customFormat="false" ht="23.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A170" s="4" t="s">
+        <v>211</v>
+      </c>
+      <c r="B170" s="4" t="s">
+        <v>213</v>
+      </c>
+      <c r="C170" s="4" t="n">
+        <v>0.7775882</v>
+      </c>
+      <c r="D170" s="4" t="n">
+        <v>0.6686706</v>
+      </c>
+      <c r="E170" s="4" t="n">
+        <v>0.6176222</v>
+      </c>
+      <c r="F170" s="4" t="n">
+        <v>1.8428388</v>
+      </c>
+      <c r="G170" s="4" t="n">
+        <v>0.90282</v>
+      </c>
+      <c r="H170" s="4"/>
+      <c r="I170" s="4"/>
+    </row>
+    <row r="171" customFormat="false" ht="23.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A171" s="4" t="s">
+        <v>211</v>
+      </c>
+      <c r="B171" s="4" t="s">
+        <v>214</v>
+      </c>
+      <c r="C171" s="4" t="n">
+        <v>0.815509</v>
+      </c>
+      <c r="D171" s="4" t="n">
+        <v>0.7471458</v>
+      </c>
+      <c r="E171" s="4" t="n">
+        <v>0.8018268</v>
+      </c>
+      <c r="F171" s="4" t="n">
+        <v>2.0695492</v>
+      </c>
+      <c r="G171" s="4" t="n">
+        <v>1.2676812</v>
+      </c>
+      <c r="H171" s="4"/>
+      <c r="I171" s="4"/>
+    </row>
+    <row r="172" customFormat="false" ht="23.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A172" s="4" t="s">
+        <v>215</v>
+      </c>
+      <c r="B172" s="4" t="s">
+        <v>216</v>
+      </c>
+      <c r="C172" s="4" t="n">
+        <v>0.4162216</v>
+      </c>
+      <c r="D172" s="4" t="n">
+        <v>0.383837</v>
+      </c>
+      <c r="E172" s="4" t="n">
+        <v>0.3766196</v>
+      </c>
+      <c r="F172" s="4" t="n">
+        <v>1.0861074</v>
+      </c>
+      <c r="G172" s="4" t="n">
+        <v>0.4103676</v>
+      </c>
+      <c r="H172" s="4"/>
+      <c r="I172" s="4"/>
+    </row>
+    <row r="173" customFormat="false" ht="23.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A173" s="4" t="s">
+        <v>215</v>
+      </c>
+      <c r="B173" s="4" t="s">
+        <v>217</v>
+      </c>
+      <c r="C173" s="4" t="n">
+        <v>0.3052626</v>
+      </c>
+      <c r="D173" s="4" t="n">
+        <v>0.3391674</v>
+      </c>
+      <c r="E173" s="4" t="n">
+        <v>0.29671</v>
+      </c>
+      <c r="F173" s="4" t="n">
+        <v>1.1355016</v>
+      </c>
+      <c r="G173" s="4" t="n">
+        <v>0.3405168</v>
+      </c>
+      <c r="H173" s="4"/>
+      <c r="I173" s="4"/>
+    </row>
+    <row r="174" customFormat="false" ht="23.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A174" s="4" t="s">
+        <v>215</v>
+      </c>
+      <c r="B174" s="4" t="s">
+        <v>218</v>
+      </c>
+      <c r="C174" s="4" t="n">
+        <v>0.3732976</v>
+      </c>
+      <c r="D174" s="4" t="n">
+        <v>0.3428344</v>
+      </c>
+      <c r="E174" s="4" t="n">
+        <v>0.3121602</v>
+      </c>
+      <c r="F174" s="4" t="n">
+        <v>1.1046554</v>
+      </c>
+      <c r="G174" s="4" t="n">
+        <v>0.3802564</v>
+      </c>
+      <c r="H174" s="4"/>
+      <c r="I174" s="4"/>
+    </row>
+    <row r="175" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A175" s="4" t="s">
+        <v>215</v>
+      </c>
+      <c r="B175" s="4" t="s">
+        <v>219</v>
+      </c>
+      <c r="C175" s="4" t="n">
+        <v>0.365924</v>
+      </c>
+      <c r="D175" s="4" t="n">
+        <v>0.3441764</v>
+      </c>
+      <c r="E175" s="4" t="n">
+        <v>0.3574002</v>
+      </c>
+      <c r="F175" s="4" t="n">
+        <v>1.0996522</v>
+      </c>
+      <c r="G175" s="4" t="n">
+        <v>0.4002544</v>
+      </c>
+      <c r="H175" s="4"/>
+      <c r="I175" s="4"/>
+    </row>
+    <row r="176" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A176" s="4" t="s">
+        <v>215</v>
+      </c>
+      <c r="B176" s="4" t="s">
+        <v>220</v>
+      </c>
+      <c r="C176" s="4" t="n">
+        <v>0.4314106</v>
+      </c>
+      <c r="D176" s="4" t="n">
+        <v>0.358788</v>
+      </c>
+      <c r="E176" s="4" t="n">
+        <v>0.3772826</v>
+      </c>
+      <c r="F176" s="4" t="n">
+        <v>1.144587</v>
+      </c>
+      <c r="G176" s="4" t="n">
+        <v>0.48563</v>
+      </c>
+      <c r="H176" s="4"/>
+      <c r="I176" s="4"/>
+    </row>
+    <row r="177" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A177" s="4" t="s">
+        <v>215</v>
+      </c>
+      <c r="B177" s="4" t="s">
+        <v>221</v>
+      </c>
+      <c r="C177" s="4" t="n">
+        <v>0.4433452</v>
+      </c>
+      <c r="D177" s="4" t="n">
+        <v>0.3827698</v>
+      </c>
+      <c r="E177" s="4" t="n">
+        <v>0.3570656</v>
+      </c>
+      <c r="F177" s="4" t="n">
+        <v>1.1826044</v>
+      </c>
+      <c r="G177" s="4" t="n">
+        <v>0.3923944</v>
+      </c>
+      <c r="H177" s="4"/>
+      <c r="I177" s="4"/>
+    </row>
+    <row r="178" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A178" s="4" t="s">
+        <v>222</v>
+      </c>
+      <c r="B178" s="4" t="s">
+        <v>223</v>
+      </c>
+      <c r="C178" s="4" t="n">
+        <v>0.4696164</v>
+      </c>
+      <c r="D178" s="4" t="n">
+        <v>0.3848094</v>
+      </c>
+      <c r="E178" s="4" t="n">
+        <v>0.4176626</v>
+      </c>
+      <c r="F178" s="4" t="n">
+        <v>1.1840152</v>
+      </c>
+      <c r="G178" s="4" t="n">
+        <v>0.441146</v>
+      </c>
+      <c r="H178" s="4"/>
+      <c r="I178" s="4"/>
+    </row>
+    <row r="179" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A179" s="4" t="s">
+        <v>222</v>
+      </c>
+      <c r="B179" s="4" t="s">
+        <v>224</v>
+      </c>
+      <c r="C179" s="4" t="n">
+        <v>0.410679</v>
+      </c>
+      <c r="D179" s="4" t="n">
+        <v>0.3448572</v>
+      </c>
+      <c r="E179" s="4" t="n">
+        <v>0.352888</v>
+      </c>
+      <c r="F179" s="4" t="n">
+        <v>1.1461254</v>
+      </c>
+      <c r="G179" s="4" t="n">
+        <v>0.3651974</v>
+      </c>
+      <c r="H179" s="4"/>
+      <c r="I179" s="4"/>
+    </row>
+    <row r="180" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A180" s="4" t="s">
+        <v>222</v>
+      </c>
+      <c r="B180" s="4" t="s">
+        <v>225</v>
+      </c>
+      <c r="C180" s="4" t="n">
+        <v>0.3621034</v>
+      </c>
+      <c r="D180" s="4" t="n">
+        <v>0.3653964</v>
+      </c>
+      <c r="E180" s="4" t="n">
+        <v>0.3950768</v>
+      </c>
+      <c r="F180" s="4" t="n">
+        <v>1.3053016</v>
+      </c>
+      <c r="G180" s="4" t="n">
+        <v>0.3838866</v>
+      </c>
+      <c r="H180" s="4"/>
+      <c r="I180" s="4"/>
     </row>
     <row r="1048560" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="1048561" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -5961,8 +6361,8 @@
   </sheetPr>
   <dimension ref="A1:I1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A151" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B164" activeCellId="0" sqref="B164"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A169" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D184" activeCellId="0" sqref="D184"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -6006,7 +6406,7 @@
         <v>11</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>210</v>
+        <v>226</v>
       </c>
       <c r="C2" s="4" t="n">
         <v>2.0220664</v>
@@ -6029,7 +6429,7 @@
         <v>11</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>211</v>
+        <v>227</v>
       </c>
       <c r="C3" s="4" t="n">
         <v>2.4586498</v>
@@ -6075,7 +6475,7 @@
         <v>15</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>212</v>
+        <v>228</v>
       </c>
       <c r="C5" s="4" t="n">
         <v>2.1296676</v>
@@ -6144,7 +6544,7 @@
         <v>19</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>213</v>
+        <v>229</v>
       </c>
       <c r="C8" s="4" t="n">
         <v>2.1709282</v>
@@ -6167,7 +6567,7 @@
         <v>19</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>214</v>
+        <v>230</v>
       </c>
       <c r="C9" s="4" t="n">
         <v>2.1589454</v>
@@ -6190,7 +6590,7 @@
         <v>19</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>215</v>
+        <v>231</v>
       </c>
       <c r="C10" s="4" t="n">
         <v>2.0390428</v>
@@ -6236,7 +6636,7 @@
         <v>23</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>216</v>
+        <v>232</v>
       </c>
       <c r="C12" s="4" t="n">
         <v>1.9875636</v>
@@ -6305,7 +6705,7 @@
         <v>27</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>217</v>
+        <v>233</v>
       </c>
       <c r="C15" s="4" t="n">
         <v>2.1964826</v>
@@ -6512,7 +6912,7 @@
         <v>39</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>218</v>
+        <v>234</v>
       </c>
       <c r="C24" s="4" t="n">
         <v>2.6861386</v>
@@ -6558,7 +6958,7 @@
         <v>39</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>219</v>
+        <v>235</v>
       </c>
       <c r="C26" s="4" t="n">
         <v>2.330873</v>
@@ -6581,7 +6981,7 @@
         <v>39</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>220</v>
+        <v>236</v>
       </c>
       <c r="C27" s="4" t="n">
         <v>2.4523078</v>
@@ -6604,7 +7004,7 @@
         <v>39</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>221</v>
+        <v>237</v>
       </c>
       <c r="C28" s="4" t="n">
         <v>2.3690538</v>
@@ -6650,7 +7050,7 @@
         <v>46</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>222</v>
+        <v>238</v>
       </c>
       <c r="C30" s="4" t="n">
         <v>2.3269536</v>
@@ -6696,7 +7096,7 @@
         <v>50</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>223</v>
+        <v>239</v>
       </c>
       <c r="C32" s="4" t="n">
         <v>1.9277496</v>
@@ -6788,7 +7188,7 @@
         <v>53</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>212</v>
+        <v>228</v>
       </c>
       <c r="C36" s="4" t="n">
         <v>2.1296676</v>
@@ -6834,7 +7234,7 @@
         <v>56</v>
       </c>
       <c r="B38" s="4" t="s">
-        <v>224</v>
+        <v>240</v>
       </c>
       <c r="C38" s="4" t="n">
         <v>2.138844</v>
@@ -6857,7 +7257,7 @@
         <v>56</v>
       </c>
       <c r="B39" s="4" t="s">
-        <v>225</v>
+        <v>241</v>
       </c>
       <c r="C39" s="4" t="n">
         <v>2.569399</v>
@@ -6880,7 +7280,7 @@
         <v>56</v>
       </c>
       <c r="B40" s="4" t="s">
-        <v>226</v>
+        <v>242</v>
       </c>
       <c r="C40" s="4" t="n">
         <v>2.2719068</v>
@@ -6903,7 +7303,7 @@
         <v>60</v>
       </c>
       <c r="B41" s="4" t="s">
-        <v>227</v>
+        <v>243</v>
       </c>
       <c r="C41" s="4" t="n">
         <v>2.4505342</v>
@@ -6926,7 +7326,7 @@
         <v>60</v>
       </c>
       <c r="B42" s="4" t="s">
-        <v>228</v>
+        <v>244</v>
       </c>
       <c r="C42" s="4" t="n">
         <v>2.5803136</v>
@@ -6972,7 +7372,7 @@
         <v>64</v>
       </c>
       <c r="B44" s="4" t="s">
-        <v>229</v>
+        <v>245</v>
       </c>
       <c r="C44" s="4" t="n">
         <v>2.4560934</v>
@@ -6995,7 +7395,7 @@
         <v>64</v>
       </c>
       <c r="B45" s="4" t="s">
-        <v>230</v>
+        <v>246</v>
       </c>
       <c r="C45" s="4" t="n">
         <v>2.0923624</v>
@@ -7018,7 +7418,7 @@
         <v>64</v>
       </c>
       <c r="B46" s="4" t="s">
-        <v>231</v>
+        <v>247</v>
       </c>
       <c r="C46" s="4" t="n">
         <v>2.7843442</v>
@@ -7271,7 +7671,7 @@
         <v>80</v>
       </c>
       <c r="B57" s="4" t="s">
-        <v>232</v>
+        <v>248</v>
       </c>
       <c r="C57" s="4" t="n">
         <v>2.9062288</v>
@@ -7478,7 +7878,7 @@
         <v>91</v>
       </c>
       <c r="B66" s="4" t="s">
-        <v>233</v>
+        <v>249</v>
       </c>
       <c r="C66" s="4" t="n">
         <v>3.3981744</v>
@@ -7501,7 +7901,7 @@
         <v>91</v>
       </c>
       <c r="B67" s="4" t="s">
-        <v>234</v>
+        <v>250</v>
       </c>
       <c r="C67" s="4" t="n">
         <v>2.0062282</v>
@@ -7524,7 +7924,7 @@
         <v>95</v>
       </c>
       <c r="B68" s="4" t="s">
-        <v>235</v>
+        <v>251</v>
       </c>
       <c r="C68" s="4" t="n">
         <v>5.4740242</v>
@@ -7547,7 +7947,7 @@
         <v>95</v>
       </c>
       <c r="B69" s="4" t="s">
-        <v>236</v>
+        <v>252</v>
       </c>
       <c r="C69" s="4" t="n">
         <v>5.0492016</v>
@@ -7685,7 +8085,7 @@
         <v>103</v>
       </c>
       <c r="B75" s="4" t="s">
-        <v>222</v>
+        <v>238</v>
       </c>
       <c r="C75" s="4" t="n">
         <v>2.7314032</v>
@@ -7708,7 +8108,7 @@
         <v>103</v>
       </c>
       <c r="B76" s="4" t="s">
-        <v>237</v>
+        <v>253</v>
       </c>
       <c r="C76" s="4" t="n">
         <v>2.7375454</v>
@@ -7777,7 +8177,7 @@
         <v>107</v>
       </c>
       <c r="B79" s="4" t="s">
-        <v>238</v>
+        <v>254</v>
       </c>
       <c r="C79" s="4" t="n">
         <v>2.5848074</v>
@@ -7984,7 +8384,7 @@
         <v>118</v>
       </c>
       <c r="B88" s="4" t="s">
-        <v>214</v>
+        <v>230</v>
       </c>
       <c r="C88" s="4" t="n">
         <v>1.9251046</v>
@@ -8007,7 +8407,7 @@
         <v>122</v>
       </c>
       <c r="B89" s="4" t="s">
-        <v>212</v>
+        <v>228</v>
       </c>
       <c r="C89" s="4" t="n">
         <v>2.1296676</v>
@@ -8076,7 +8476,7 @@
         <v>126</v>
       </c>
       <c r="B92" s="4" t="s">
-        <v>239</v>
+        <v>255</v>
       </c>
       <c r="C92" s="4" t="n">
         <v>2.543308</v>
@@ -8099,7 +8499,7 @@
         <v>126</v>
       </c>
       <c r="B93" s="4" t="s">
-        <v>240</v>
+        <v>256</v>
       </c>
       <c r="C93" s="4" t="n">
         <v>2.6339666</v>
@@ -8122,7 +8522,7 @@
         <v>126</v>
       </c>
       <c r="B94" s="4" t="s">
-        <v>214</v>
+        <v>230</v>
       </c>
       <c r="C94" s="4" t="n">
         <v>2.4568346</v>
@@ -8260,7 +8660,7 @@
         <v>131</v>
       </c>
       <c r="B100" s="4" t="s">
-        <v>232</v>
+        <v>248</v>
       </c>
       <c r="C100" s="4" t="n">
         <v>2.403287</v>
@@ -8306,7 +8706,7 @@
         <v>134</v>
       </c>
       <c r="B102" s="4" t="s">
-        <v>241</v>
+        <v>257</v>
       </c>
       <c r="C102" s="4" t="n">
         <v>3.021798</v>
@@ -8421,7 +8821,7 @@
         <v>139</v>
       </c>
       <c r="B107" s="4" t="s">
-        <v>216</v>
+        <v>232</v>
       </c>
       <c r="C107" s="4" t="n">
         <v>2.208845</v>
@@ -8605,7 +9005,7 @@
         <v>144</v>
       </c>
       <c r="B115" s="4" t="s">
-        <v>242</v>
+        <v>258</v>
       </c>
       <c r="C115" s="4" t="n">
         <v>2.1219888</v>
@@ -8697,7 +9097,7 @@
         <v>152</v>
       </c>
       <c r="B119" s="4" t="s">
-        <v>243</v>
+        <v>259</v>
       </c>
       <c r="C119" s="4" t="n">
         <v>2.5949094</v>
@@ -8743,7 +9143,7 @@
         <v>152</v>
       </c>
       <c r="B121" s="4" t="s">
-        <v>244</v>
+        <v>260</v>
       </c>
       <c r="C121" s="4" t="n">
         <v>1.9941926</v>
@@ -8766,7 +9166,7 @@
         <v>156</v>
       </c>
       <c r="B122" s="4" t="s">
-        <v>245</v>
+        <v>261</v>
       </c>
       <c r="C122" s="4" t="n">
         <v>2.4594108</v>
@@ -8950,7 +9350,7 @@
         <v>164</v>
       </c>
       <c r="B130" s="4" t="s">
-        <v>246</v>
+        <v>262</v>
       </c>
       <c r="C130" s="4" t="n">
         <v>1.9619838</v>
@@ -9019,7 +9419,7 @@
         <v>169</v>
       </c>
       <c r="B133" s="4" t="s">
-        <v>247</v>
+        <v>263</v>
       </c>
       <c r="C133" s="4" t="n">
         <v>1.8671148</v>
@@ -9349,7 +9749,7 @@
         <v>184</v>
       </c>
       <c r="B147" s="4" t="s">
-        <v>248</v>
+        <v>264</v>
       </c>
       <c r="C147" s="4" t="n">
         <v>3.166509</v>
@@ -9374,7 +9774,7 @@
         <v>184</v>
       </c>
       <c r="B148" s="4" t="s">
-        <v>214</v>
+        <v>230</v>
       </c>
       <c r="C148" s="4" t="n">
         <v>3.119118</v>
@@ -9399,7 +9799,7 @@
         <v>184</v>
       </c>
       <c r="B149" s="4" t="s">
-        <v>249</v>
+        <v>265</v>
       </c>
       <c r="C149" s="4" t="n">
         <v>2.901321</v>
@@ -9744,12 +10144,12 @@
       <c r="H162" s="4"/>
       <c r="I162" s="4"/>
     </row>
-    <row r="163" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="163" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A163" s="4" t="s">
         <v>203</v>
       </c>
       <c r="B163" s="4" t="s">
-        <v>250</v>
+        <v>266</v>
       </c>
       <c r="C163" s="4" t="n">
         <v>2.0239208</v>
@@ -9769,7 +10169,7 @@
       <c r="H163" s="4"/>
       <c r="I163" s="4"/>
     </row>
-    <row r="164" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="164" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A164" s="4" t="s">
         <v>203</v>
       </c>
@@ -9794,7 +10194,7 @@
       <c r="H164" s="4"/>
       <c r="I164" s="4"/>
     </row>
-    <row r="165" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="165" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A165" s="4" t="s">
         <v>203</v>
       </c>
@@ -9819,7 +10219,7 @@
       <c r="H165" s="4"/>
       <c r="I165" s="4"/>
     </row>
-    <row r="166" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="166" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A166" s="4" t="s">
         <v>207</v>
       </c>
@@ -9844,12 +10244,12 @@
       <c r="H166" s="4"/>
       <c r="I166" s="4"/>
     </row>
-    <row r="167" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="167" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A167" s="4" t="s">
         <v>207</v>
       </c>
       <c r="B167" s="4" t="s">
-        <v>251</v>
+        <v>267</v>
       </c>
       <c r="C167" s="4" t="n">
         <v>1.8280256</v>
@@ -9869,7 +10269,7 @@
       <c r="H167" s="4"/>
       <c r="I167" s="4"/>
     </row>
-    <row r="168" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="168" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A168" s="4" t="s">
         <v>207</v>
       </c>
@@ -9893,6 +10293,356 @@
       </c>
       <c r="H168" s="4"/>
       <c r="I168" s="4"/>
+    </row>
+    <row r="169" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A169" s="4" t="s">
+        <v>211</v>
+      </c>
+      <c r="B169" s="4" t="s">
+        <v>212</v>
+      </c>
+      <c r="C169" s="4" t="n">
+        <v>2.1684784</v>
+      </c>
+      <c r="D169" s="4" t="n">
+        <v>3.6719008</v>
+      </c>
+      <c r="E169" s="4" t="n">
+        <v>0.8740194</v>
+      </c>
+      <c r="F169" s="4" t="n">
+        <v>2.3532634</v>
+      </c>
+      <c r="G169" s="4" t="n">
+        <v>0.9487852</v>
+      </c>
+      <c r="H169" s="4"/>
+      <c r="I169" s="4"/>
+    </row>
+    <row r="170" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A170" s="4" t="s">
+        <v>211</v>
+      </c>
+      <c r="B170" s="4" t="s">
+        <v>213</v>
+      </c>
+      <c r="C170" s="4" t="n">
+        <v>2.6452654</v>
+      </c>
+      <c r="D170" s="4" t="n">
+        <v>3.6146782</v>
+      </c>
+      <c r="E170" s="4" t="n">
+        <v>1.6826424</v>
+      </c>
+      <c r="F170" s="4" t="n">
+        <v>2.2919798</v>
+      </c>
+      <c r="G170" s="4" t="n">
+        <v>1.1919476</v>
+      </c>
+      <c r="H170" s="4"/>
+      <c r="I170" s="4"/>
+    </row>
+    <row r="171" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A171" s="4" t="s">
+        <v>211</v>
+      </c>
+      <c r="B171" s="4" t="s">
+        <v>259</v>
+      </c>
+      <c r="C171" s="4" t="n">
+        <v>3.5371194</v>
+      </c>
+      <c r="D171" s="4" t="n">
+        <v>2.6826182</v>
+      </c>
+      <c r="E171" s="4" t="n">
+        <v>1.985354</v>
+      </c>
+      <c r="F171" s="4" t="n">
+        <v>2.852045</v>
+      </c>
+      <c r="G171" s="4" t="n">
+        <v>1.5791478</v>
+      </c>
+      <c r="H171" s="4"/>
+      <c r="I171" s="4"/>
+    </row>
+    <row r="172" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A172" s="4" t="s">
+        <v>215</v>
+      </c>
+      <c r="B172" s="4" t="s">
+        <v>216</v>
+      </c>
+      <c r="C172" s="4" t="n">
+        <v>1.8111492</v>
+      </c>
+      <c r="D172" s="4" t="n">
+        <v>3.5453204</v>
+      </c>
+      <c r="E172" s="4" t="n">
+        <v>4.565067</v>
+      </c>
+      <c r="F172" s="4" t="n">
+        <v>5.155638</v>
+      </c>
+      <c r="G172" s="4" t="n">
+        <v>3.3921948</v>
+      </c>
+      <c r="H172" s="4"/>
+      <c r="I172" s="4"/>
+    </row>
+    <row r="173" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A173" s="4" t="s">
+        <v>215</v>
+      </c>
+      <c r="B173" s="4" t="s">
+        <v>218</v>
+      </c>
+      <c r="C173" s="4" t="n">
+        <v>2.003195</v>
+      </c>
+      <c r="D173" s="4" t="n">
+        <v>3.988986</v>
+      </c>
+      <c r="E173" s="4" t="n">
+        <v>4.3174654</v>
+      </c>
+      <c r="F173" s="4" t="n">
+        <v>5.0137714</v>
+      </c>
+      <c r="G173" s="4" t="n">
+        <v>3.3907598</v>
+      </c>
+      <c r="H173" s="4"/>
+      <c r="I173" s="4"/>
+    </row>
+    <row r="174" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A174" s="4" t="s">
+        <v>215</v>
+      </c>
+      <c r="B174" s="4" t="s">
+        <v>268</v>
+      </c>
+      <c r="C174" s="4" t="n">
+        <v>1.8331202</v>
+      </c>
+      <c r="D174" s="4" t="n">
+        <v>3.9389388</v>
+      </c>
+      <c r="E174" s="4" t="n">
+        <v>4.3728444</v>
+      </c>
+      <c r="F174" s="4" t="n">
+        <v>4.9377702</v>
+      </c>
+      <c r="G174" s="4" t="n">
+        <v>3.3644016</v>
+      </c>
+      <c r="H174" s="4"/>
+      <c r="I174" s="4"/>
+    </row>
+    <row r="175" customFormat="false" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A175" s="4" t="s">
+        <v>215</v>
+      </c>
+      <c r="B175" s="4" t="s">
+        <v>219</v>
+      </c>
+      <c r="C175" s="4" t="n">
+        <v>2.0748002</v>
+      </c>
+      <c r="D175" s="4" t="n">
+        <v>6.1653436</v>
+      </c>
+      <c r="E175" s="4" t="n">
+        <v>4.6023164</v>
+      </c>
+      <c r="F175" s="4" t="n">
+        <v>5.0471982</v>
+      </c>
+      <c r="G175" s="4" t="n">
+        <v>3.4146058</v>
+      </c>
+      <c r="H175" s="4"/>
+      <c r="I175" s="4"/>
+    </row>
+    <row r="176" customFormat="false" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A176" s="4" t="s">
+        <v>215</v>
+      </c>
+      <c r="B176" s="4" t="s">
+        <v>269</v>
+      </c>
+      <c r="C176" s="4" t="n">
+        <v>1.8676058</v>
+      </c>
+      <c r="D176" s="4" t="n">
+        <v>3.9589414</v>
+      </c>
+      <c r="E176" s="4" t="n">
+        <v>4.3995558</v>
+      </c>
+      <c r="F176" s="4" t="n">
+        <v>5.1930024</v>
+      </c>
+      <c r="G176" s="4" t="n">
+        <v>3.4905538</v>
+      </c>
+      <c r="H176" s="4"/>
+      <c r="I176" s="4"/>
+    </row>
+    <row r="177" customFormat="false" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A177" s="4" t="s">
+        <v>215</v>
+      </c>
+      <c r="B177" s="4" t="s">
+        <v>270</v>
+      </c>
+      <c r="C177" s="4" t="n">
+        <v>1.8565564</v>
+      </c>
+      <c r="D177" s="4" t="n">
+        <v>4.0912932</v>
+      </c>
+      <c r="E177" s="4" t="n">
+        <v>4.4175284</v>
+      </c>
+      <c r="F177" s="4" t="n">
+        <v>5.099716</v>
+      </c>
+      <c r="G177" s="4" t="n">
+        <v>3.5278338</v>
+      </c>
+      <c r="H177" s="4"/>
+      <c r="I177" s="4"/>
+    </row>
+    <row r="178" customFormat="false" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A178" s="4" t="s">
+        <v>215</v>
+      </c>
+      <c r="B178" s="4" t="s">
+        <v>271</v>
+      </c>
+      <c r="C178" s="4" t="n">
+        <v>1.971548</v>
+      </c>
+      <c r="D178" s="4" t="n">
+        <v>3.9851468</v>
+      </c>
+      <c r="E178" s="4" t="n">
+        <v>4.3151926</v>
+      </c>
+      <c r="F178" s="4" t="n">
+        <v>5.217876</v>
+      </c>
+      <c r="G178" s="4" t="n">
+        <v>3.4074138</v>
+      </c>
+      <c r="H178" s="4"/>
+      <c r="I178" s="4"/>
+    </row>
+    <row r="179" customFormat="false" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A179" s="4" t="s">
+        <v>215</v>
+      </c>
+      <c r="B179" s="4" t="s">
+        <v>272</v>
+      </c>
+      <c r="C179" s="4" t="n">
+        <v>1.8706844</v>
+      </c>
+      <c r="D179" s="4" t="n">
+        <v>3.9432928</v>
+      </c>
+      <c r="E179" s="4" t="n">
+        <v>4.358427</v>
+      </c>
+      <c r="F179" s="4" t="n">
+        <v>5.1559578</v>
+      </c>
+      <c r="G179" s="4" t="n">
+        <v>3.3936074</v>
+      </c>
+      <c r="H179" s="4"/>
+      <c r="I179" s="4"/>
+    </row>
+    <row r="180" customFormat="false" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A180" s="4" t="s">
+        <v>222</v>
+      </c>
+      <c r="B180" s="4" t="s">
+        <v>223</v>
+      </c>
+      <c r="C180" s="4" t="n">
+        <v>2.0217014</v>
+      </c>
+      <c r="D180" s="4" t="n">
+        <v>3.767755</v>
+      </c>
+      <c r="E180" s="4" t="n">
+        <v>4.6003578</v>
+      </c>
+      <c r="F180" s="4" t="n">
+        <v>5.4023852</v>
+      </c>
+      <c r="G180" s="4" t="n">
+        <v>3.3677646</v>
+      </c>
+      <c r="H180" s="4"/>
+      <c r="I180" s="4"/>
+    </row>
+    <row r="181" customFormat="false" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A181" s="4" t="s">
+        <v>222</v>
+      </c>
+      <c r="B181" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="C181" s="4" t="n">
+        <v>2.240086</v>
+      </c>
+      <c r="D181" s="4" t="n">
+        <v>3.9737116</v>
+      </c>
+      <c r="E181" s="4" t="n">
+        <v>4.3489156</v>
+      </c>
+      <c r="F181" s="4" t="n">
+        <v>5.0343732</v>
+      </c>
+      <c r="G181" s="4" t="n">
+        <v>3.8793686</v>
+      </c>
+      <c r="H181" s="4"/>
+      <c r="I181" s="4"/>
+    </row>
+    <row r="182" customFormat="false" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A182" s="4" t="s">
+        <v>222</v>
+      </c>
+      <c r="B182" s="4" t="s">
+        <v>273</v>
+      </c>
+      <c r="C182" s="4" t="n">
+        <v>2.0147578</v>
+      </c>
+      <c r="D182" s="4" t="n">
+        <v>4.0021432</v>
+      </c>
+      <c r="E182" s="4" t="n">
+        <v>4.3717046</v>
+      </c>
+      <c r="F182" s="4" t="n">
+        <v>4.9437112</v>
+      </c>
+      <c r="G182" s="4" t="n">
+        <v>3.551135</v>
+      </c>
+      <c r="H182" s="4"/>
+      <c r="I182" s="4"/>
     </row>
     <row r="1048562" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="1048563" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -9927,8 +10677,8 @@
   </sheetPr>
   <dimension ref="A1:I1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A151" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A162" activeCellId="0" sqref="A162"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A166" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D177" activeCellId="0" sqref="D177"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -9972,7 +10722,7 @@
         <v>11</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>252</v>
+        <v>274</v>
       </c>
       <c r="C2" s="4" t="n">
         <v>0.7804054</v>
@@ -9995,7 +10745,7 @@
         <v>11</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>253</v>
+        <v>275</v>
       </c>
       <c r="C3" s="4" t="n">
         <v>0.7779802</v>
@@ -10018,7 +10768,7 @@
         <v>11</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>254</v>
+        <v>276</v>
       </c>
       <c r="C4" s="4" t="n">
         <v>0.7043458</v>
@@ -10041,7 +10791,7 @@
         <v>15</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>255</v>
+        <v>277</v>
       </c>
       <c r="C5" s="4" t="n">
         <v>0.7145706</v>
@@ -10110,7 +10860,7 @@
         <v>19</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>213</v>
+        <v>229</v>
       </c>
       <c r="C8" s="4" t="n">
         <v>0.6280168</v>
@@ -10156,7 +10906,7 @@
         <v>19</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>256</v>
+        <v>278</v>
       </c>
       <c r="C10" s="4" t="n">
         <v>0.7373706</v>
@@ -10202,7 +10952,7 @@
         <v>23</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>216</v>
+        <v>232</v>
       </c>
       <c r="C12" s="4" t="n">
         <v>0.7234852</v>
@@ -10294,7 +11044,7 @@
         <v>27</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>257</v>
+        <v>279</v>
       </c>
       <c r="C16" s="4" t="n">
         <v>0.3510038</v>
@@ -10340,7 +11090,7 @@
         <v>31</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>258</v>
+        <v>216</v>
       </c>
       <c r="C18" s="4" t="n">
         <v>0.5591408</v>
@@ -10363,7 +11113,7 @@
         <v>31</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>259</v>
+        <v>280</v>
       </c>
       <c r="C19" s="4" t="n">
         <v>0.5551518</v>
@@ -10455,7 +11205,7 @@
         <v>39</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>260</v>
+        <v>281</v>
       </c>
       <c r="C23" s="4" t="n">
         <v>0.9795414</v>
@@ -10478,7 +11228,7 @@
         <v>39</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>261</v>
+        <v>282</v>
       </c>
       <c r="C24" s="4" t="n">
         <v>3.7305486</v>
@@ -10501,7 +11251,7 @@
         <v>39</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>262</v>
+        <v>283</v>
       </c>
       <c r="C25" s="4" t="n">
         <v>2.3842444</v>
@@ -10524,7 +11274,7 @@
         <v>39</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>263</v>
+        <v>284</v>
       </c>
       <c r="C26" s="4" t="n">
         <v>2.139728</v>
@@ -10547,7 +11297,7 @@
         <v>39</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>264</v>
+        <v>285</v>
       </c>
       <c r="C27" s="4" t="n">
         <v>0.7112716</v>
@@ -10570,7 +11320,7 @@
         <v>39</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>265</v>
+        <v>286</v>
       </c>
       <c r="C28" s="4" t="n">
         <v>0.67812</v>
@@ -10616,7 +11366,7 @@
         <v>46</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>266</v>
+        <v>287</v>
       </c>
       <c r="C30" s="4" t="n">
         <v>0.712753</v>
@@ -10639,7 +11389,7 @@
         <v>46</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>267</v>
+        <v>288</v>
       </c>
       <c r="C31" s="4" t="n">
         <v>0.630812</v>
@@ -10685,7 +11435,7 @@
         <v>50</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>268</v>
+        <v>289</v>
       </c>
       <c r="C33" s="4" t="n">
         <v>0.7013216</v>
@@ -10754,7 +11504,7 @@
         <v>53</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>254</v>
+        <v>276</v>
       </c>
       <c r="C36" s="4" t="n">
         <v>0.7043458</v>
@@ -10777,7 +11527,7 @@
         <v>53</v>
       </c>
       <c r="B37" s="4" t="s">
-        <v>255</v>
+        <v>277</v>
       </c>
       <c r="C37" s="4" t="n">
         <v>0.7145706</v>
@@ -10800,7 +11550,7 @@
         <v>56</v>
       </c>
       <c r="B38" s="4" t="s">
-        <v>269</v>
+        <v>290</v>
       </c>
       <c r="C38" s="4" t="n">
         <v>1.2584274</v>
@@ -10823,7 +11573,7 @@
         <v>56</v>
       </c>
       <c r="B39" s="4" t="s">
-        <v>270</v>
+        <v>291</v>
       </c>
       <c r="C39" s="4" t="n">
         <v>1.3856258</v>
@@ -10846,7 +11596,7 @@
         <v>56</v>
       </c>
       <c r="B40" s="4" t="s">
-        <v>271</v>
+        <v>292</v>
       </c>
       <c r="C40" s="4" t="n">
         <v>1.1413118</v>
@@ -10869,7 +11619,7 @@
         <v>60</v>
       </c>
       <c r="B41" s="4" t="s">
-        <v>272</v>
+        <v>293</v>
       </c>
       <c r="C41" s="4" t="n">
         <v>2.0516946</v>
@@ -10938,7 +11688,7 @@
         <v>64</v>
       </c>
       <c r="B44" s="4" t="s">
-        <v>273</v>
+        <v>294</v>
       </c>
       <c r="C44" s="4" t="n">
         <v>0.7883284</v>
@@ -10984,7 +11734,7 @@
         <v>64</v>
       </c>
       <c r="B46" s="4" t="s">
-        <v>274</v>
+        <v>295</v>
       </c>
       <c r="C46" s="4" t="n">
         <v>0.6814198</v>
@@ -11099,7 +11849,7 @@
         <v>72</v>
       </c>
       <c r="B51" s="4" t="s">
-        <v>275</v>
+        <v>296</v>
       </c>
       <c r="C51" s="4" t="n">
         <v>1.4049502</v>
@@ -11145,7 +11895,7 @@
         <v>76</v>
       </c>
       <c r="B53" s="4" t="s">
-        <v>276</v>
+        <v>297</v>
       </c>
       <c r="C53" s="4" t="n">
         <v>0.9897652</v>
@@ -11214,7 +11964,7 @@
         <v>80</v>
       </c>
       <c r="B56" s="4" t="s">
-        <v>277</v>
+        <v>298</v>
       </c>
       <c r="C56" s="4" t="n">
         <v>1.2353042</v>
@@ -11260,7 +12010,7 @@
         <v>80</v>
       </c>
       <c r="B58" s="4" t="s">
-        <v>278</v>
+        <v>299</v>
       </c>
       <c r="C58" s="4" t="n">
         <v>1.2364662</v>
@@ -11306,7 +12056,7 @@
         <v>84</v>
       </c>
       <c r="B60" s="4" t="s">
-        <v>279</v>
+        <v>300</v>
       </c>
       <c r="C60" s="4" t="n">
         <v>1.1438926</v>
@@ -11421,7 +12171,7 @@
         <v>91</v>
       </c>
       <c r="B65" s="4" t="s">
-        <v>280</v>
+        <v>301</v>
       </c>
       <c r="C65" s="4" t="n">
         <v>1.8978822</v>
@@ -11444,7 +12194,7 @@
         <v>91</v>
       </c>
       <c r="B66" s="4" t="s">
-        <v>233</v>
+        <v>249</v>
       </c>
       <c r="C66" s="4" t="n">
         <v>1.1060998</v>
@@ -11467,7 +12217,7 @@
         <v>91</v>
       </c>
       <c r="B67" s="4" t="s">
-        <v>281</v>
+        <v>302</v>
       </c>
       <c r="C67" s="4" t="n">
         <v>1.6069744</v>
@@ -11490,7 +12240,7 @@
         <v>95</v>
       </c>
       <c r="B68" s="4" t="s">
-        <v>282</v>
+        <v>303</v>
       </c>
       <c r="C68" s="4" t="n">
         <v>1.6301784</v>
@@ -11513,7 +12263,7 @@
         <v>95</v>
       </c>
       <c r="B69" s="4" t="s">
-        <v>283</v>
+        <v>304</v>
       </c>
       <c r="C69" s="4" t="n">
         <v>1.5682082</v>
@@ -11536,7 +12286,7 @@
         <v>95</v>
       </c>
       <c r="B70" s="4" t="s">
-        <v>284</v>
+        <v>305</v>
       </c>
       <c r="C70" s="4" t="n">
         <v>1.4442308</v>
@@ -11674,7 +12424,7 @@
         <v>103</v>
       </c>
       <c r="B76" s="4" t="s">
-        <v>222</v>
+        <v>238</v>
       </c>
       <c r="C76" s="4" t="n">
         <v>1.1822766</v>
@@ -11743,7 +12493,7 @@
         <v>107</v>
       </c>
       <c r="B79" s="4" t="s">
-        <v>228</v>
+        <v>244</v>
       </c>
       <c r="C79" s="4" t="n">
         <v>1.573159</v>
@@ -12042,7 +12792,7 @@
         <v>126</v>
       </c>
       <c r="B92" s="4" t="s">
-        <v>285</v>
+        <v>306</v>
       </c>
       <c r="C92" s="4" t="n">
         <v>1.5482428</v>
@@ -12065,7 +12815,7 @@
         <v>126</v>
       </c>
       <c r="B93" s="4" t="s">
-        <v>286</v>
+        <v>307</v>
       </c>
       <c r="C93" s="4" t="n">
         <v>1.8137892</v>
@@ -12088,7 +12838,7 @@
         <v>126</v>
       </c>
       <c r="B94" s="4" t="s">
-        <v>287</v>
+        <v>308</v>
       </c>
       <c r="C94" s="4" t="n">
         <v>1.6058992</v>
@@ -12157,7 +12907,7 @@
         <v>127</v>
       </c>
       <c r="B97" s="4" t="s">
-        <v>288</v>
+        <v>309</v>
       </c>
       <c r="C97" s="4" t="n">
         <v>1.4182292</v>
@@ -12249,7 +12999,7 @@
         <v>134</v>
       </c>
       <c r="B101" s="4" t="s">
-        <v>289</v>
+        <v>310</v>
       </c>
       <c r="C101" s="4" t="n">
         <v>1.2684794</v>
@@ -12387,7 +13137,7 @@
         <v>139</v>
       </c>
       <c r="B107" s="4" t="s">
-        <v>290</v>
+        <v>311</v>
       </c>
       <c r="C107" s="4" t="n">
         <v>1.295247</v>
@@ -12410,7 +13160,7 @@
         <v>139</v>
       </c>
       <c r="B108" s="4" t="s">
-        <v>291</v>
+        <v>312</v>
       </c>
       <c r="C108" s="4" t="n">
         <v>1.22489</v>
@@ -12433,7 +13183,7 @@
         <v>139</v>
       </c>
       <c r="B109" s="4" t="s">
-        <v>292</v>
+        <v>313</v>
       </c>
       <c r="C109" s="4" t="n">
         <v>1.1823422</v>
@@ -12456,7 +13206,7 @@
         <v>142</v>
       </c>
       <c r="B110" s="4" t="s">
-        <v>293</v>
+        <v>314</v>
       </c>
       <c r="C110" s="4" t="n">
         <v>1.1176918</v>
@@ -12548,7 +13298,7 @@
         <v>144</v>
       </c>
       <c r="B114" s="4" t="s">
-        <v>242</v>
+        <v>258</v>
       </c>
       <c r="C114" s="4" t="n">
         <v>0.5937896</v>
@@ -12640,7 +13390,7 @@
         <v>148</v>
       </c>
       <c r="B118" s="4" t="s">
-        <v>294</v>
+        <v>315</v>
       </c>
       <c r="C118" s="4" t="n">
         <v>0.6148816</v>
@@ -12709,7 +13459,7 @@
         <v>152</v>
       </c>
       <c r="B121" s="4" t="s">
-        <v>244</v>
+        <v>260</v>
       </c>
       <c r="C121" s="4" t="n">
         <v>0.5689302</v>
@@ -12824,7 +13574,7 @@
         <v>160</v>
       </c>
       <c r="B126" s="4" t="s">
-        <v>267</v>
+        <v>288</v>
       </c>
       <c r="C126" s="4" t="n">
         <v>0.6197108</v>
@@ -12962,7 +13712,7 @@
         <v>169</v>
       </c>
       <c r="B132" s="4" t="s">
-        <v>295</v>
+        <v>316</v>
       </c>
       <c r="C132" s="4" t="n">
         <v>0.3808622</v>
@@ -13077,7 +13827,7 @@
         <v>169</v>
       </c>
       <c r="B137" s="4" t="s">
-        <v>280</v>
+        <v>301</v>
       </c>
       <c r="C137" s="4" t="n">
         <v>0.3914072</v>
@@ -13100,7 +13850,7 @@
         <v>169</v>
       </c>
       <c r="B138" s="4" t="s">
-        <v>296</v>
+        <v>317</v>
       </c>
       <c r="C138" s="4" t="n">
         <v>0.3957292</v>
@@ -13215,7 +13965,7 @@
         <v>182</v>
       </c>
       <c r="B143" s="4" t="s">
-        <v>255</v>
+        <v>277</v>
       </c>
       <c r="C143" s="4" t="n">
         <v>1.1999426</v>
@@ -13340,7 +14090,7 @@
         <v>184</v>
       </c>
       <c r="B148" s="4" t="s">
-        <v>297</v>
+        <v>318</v>
       </c>
       <c r="C148" s="4" t="n">
         <v>1.2852092</v>
@@ -13415,7 +14165,7 @@
         <v>189</v>
       </c>
       <c r="B151" s="4" t="s">
-        <v>298</v>
+        <v>319</v>
       </c>
       <c r="C151" s="4" t="n">
         <v>0.341044</v>
@@ -13490,7 +14240,7 @@
         <v>192</v>
       </c>
       <c r="B154" s="4" t="s">
-        <v>299</v>
+        <v>320</v>
       </c>
       <c r="C154" s="4" t="n">
         <v>0.330861</v>
@@ -13615,7 +14365,7 @@
         <v>196</v>
       </c>
       <c r="B159" s="4" t="s">
-        <v>300</v>
+        <v>321</v>
       </c>
       <c r="C159" s="4" t="n">
         <v>0.295909</v>
@@ -13685,7 +14435,7 @@
       <c r="H161" s="4"/>
       <c r="I161" s="4"/>
     </row>
-    <row r="162" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="162" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A162" s="4" t="s">
         <v>200</v>
       </c>
@@ -13710,7 +14460,7 @@
       <c r="H162" s="4"/>
       <c r="I162" s="4"/>
     </row>
-    <row r="163" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="163" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A163" s="4" t="s">
         <v>203</v>
       </c>
@@ -13735,7 +14485,7 @@
       <c r="H163" s="4"/>
       <c r="I163" s="4"/>
     </row>
-    <row r="164" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="164" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A164" s="4" t="s">
         <v>203</v>
       </c>
@@ -13760,7 +14510,7 @@
       <c r="H164" s="4"/>
       <c r="I164" s="4"/>
     </row>
-    <row r="165" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="165" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A165" s="4" t="s">
         <v>203</v>
       </c>
@@ -13785,7 +14535,7 @@
       <c r="H165" s="4"/>
       <c r="I165" s="4"/>
     </row>
-    <row r="166" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="166" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A166" s="4" t="s">
         <v>207</v>
       </c>
@@ -13810,12 +14560,12 @@
       <c r="H166" s="4"/>
       <c r="I166" s="4"/>
     </row>
-    <row r="167" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="167" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A167" s="4" t="s">
         <v>207</v>
       </c>
       <c r="B167" s="4" t="s">
-        <v>301</v>
+        <v>322</v>
       </c>
       <c r="C167" s="4" t="n">
         <v>0.4000132</v>
@@ -13835,7 +14585,7 @@
       <c r="H167" s="4"/>
       <c r="I167" s="4"/>
     </row>
-    <row r="168" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="168" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A168" s="4" t="s">
         <v>207</v>
       </c>
@@ -13859,6 +14609,306 @@
       </c>
       <c r="H168" s="4"/>
       <c r="I168" s="4"/>
+    </row>
+    <row r="169" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A169" s="4" t="s">
+        <v>211</v>
+      </c>
+      <c r="B169" s="4" t="s">
+        <v>212</v>
+      </c>
+      <c r="C169" s="4" t="n">
+        <v>0.4121864</v>
+      </c>
+      <c r="D169" s="4" t="n">
+        <v>0.3759884</v>
+      </c>
+      <c r="E169" s="4" t="n">
+        <v>0.4385392</v>
+      </c>
+      <c r="F169" s="4" t="n">
+        <v>1.1787736</v>
+      </c>
+      <c r="G169" s="4" t="n">
+        <v>0.41203</v>
+      </c>
+      <c r="H169" s="4"/>
+      <c r="I169" s="4"/>
+    </row>
+    <row r="170" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A170" s="4" t="s">
+        <v>211</v>
+      </c>
+      <c r="B170" s="4" t="s">
+        <v>213</v>
+      </c>
+      <c r="C170" s="4" t="n">
+        <v>0.898749</v>
+      </c>
+      <c r="D170" s="4" t="n">
+        <v>0.8987618</v>
+      </c>
+      <c r="E170" s="4" t="n">
+        <v>0.9598652</v>
+      </c>
+      <c r="F170" s="4" t="n">
+        <v>1.5188104</v>
+      </c>
+      <c r="G170" s="4" t="n">
+        <v>0.7639906</v>
+      </c>
+      <c r="H170" s="4"/>
+      <c r="I170" s="4"/>
+    </row>
+    <row r="171" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A171" s="4" t="s">
+        <v>211</v>
+      </c>
+      <c r="B171" s="4" t="s">
+        <v>214</v>
+      </c>
+      <c r="C171" s="4" t="n">
+        <v>0.7074952</v>
+      </c>
+      <c r="D171" s="4" t="n">
+        <v>0.8157378</v>
+      </c>
+      <c r="E171" s="4" t="n">
+        <v>0.9217552</v>
+      </c>
+      <c r="F171" s="4" t="n">
+        <v>2.2715404</v>
+      </c>
+      <c r="G171" s="4" t="n">
+        <v>1.028059</v>
+      </c>
+      <c r="H171" s="4"/>
+      <c r="I171" s="4"/>
+    </row>
+    <row r="172" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A172" s="4" t="s">
+        <v>215</v>
+      </c>
+      <c r="B172" s="4" t="s">
+        <v>323</v>
+      </c>
+      <c r="C172" s="4" t="n">
+        <v>0.3234768</v>
+      </c>
+      <c r="D172" s="4" t="n">
+        <v>0.417059</v>
+      </c>
+      <c r="E172" s="4" t="n">
+        <v>0.4604854</v>
+      </c>
+      <c r="F172" s="4" t="n">
+        <v>1.141037</v>
+      </c>
+      <c r="G172" s="4" t="n">
+        <v>0.5127828</v>
+      </c>
+      <c r="H172" s="4"/>
+      <c r="I172" s="4"/>
+    </row>
+    <row r="173" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A173" s="4" t="s">
+        <v>215</v>
+      </c>
+      <c r="B173" s="4" t="s">
+        <v>217</v>
+      </c>
+      <c r="C173" s="4" t="n">
+        <v>0.3826978</v>
+      </c>
+      <c r="D173" s="4" t="n">
+        <v>0.41345</v>
+      </c>
+      <c r="E173" s="4" t="n">
+        <v>0.4150896</v>
+      </c>
+      <c r="F173" s="4" t="n">
+        <v>1.10073</v>
+      </c>
+      <c r="G173" s="4" t="n">
+        <v>0.5701882</v>
+      </c>
+      <c r="H173" s="4"/>
+      <c r="I173" s="4"/>
+    </row>
+    <row r="174" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A174" s="4" t="s">
+        <v>215</v>
+      </c>
+      <c r="B174" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C174" s="4" t="n">
+        <v>0.3151176</v>
+      </c>
+      <c r="D174" s="4" t="n">
+        <v>0.3902366</v>
+      </c>
+      <c r="E174" s="4" t="n">
+        <v>0.4048928</v>
+      </c>
+      <c r="F174" s="4" t="n">
+        <v>1.0881796</v>
+      </c>
+      <c r="G174" s="4" t="n">
+        <v>0.4276116</v>
+      </c>
+      <c r="H174" s="4"/>
+      <c r="I174" s="4"/>
+    </row>
+    <row r="175" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A175" s="4" t="s">
+        <v>215</v>
+      </c>
+      <c r="B175" s="4" t="s">
+        <v>324</v>
+      </c>
+      <c r="C175" s="4" t="n">
+        <v>0.3166722</v>
+      </c>
+      <c r="D175" s="4" t="n">
+        <v>0.3774476</v>
+      </c>
+      <c r="E175" s="4" t="n">
+        <v>0.3556832</v>
+      </c>
+      <c r="F175" s="4" t="n">
+        <v>1.1302306</v>
+      </c>
+      <c r="G175" s="4" t="n">
+        <v>0.4634032</v>
+      </c>
+      <c r="H175" s="4"/>
+      <c r="I175" s="4"/>
+    </row>
+    <row r="176" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A176" s="4" t="s">
+        <v>215</v>
+      </c>
+      <c r="B176" s="4" t="s">
+        <v>220</v>
+      </c>
+      <c r="C176" s="4" t="n">
+        <v>0.4688078</v>
+      </c>
+      <c r="D176" s="4" t="n">
+        <v>0.4535022</v>
+      </c>
+      <c r="E176" s="4" t="n">
+        <v>0.3912784</v>
+      </c>
+      <c r="F176" s="4" t="n">
+        <v>1.0716768</v>
+      </c>
+      <c r="G176" s="4" t="n">
+        <v>0.4083036</v>
+      </c>
+      <c r="H176" s="4"/>
+      <c r="I176" s="4"/>
+    </row>
+    <row r="177" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A177" s="4" t="s">
+        <v>215</v>
+      </c>
+      <c r="B177" s="4" t="s">
+        <v>269</v>
+      </c>
+      <c r="C177" s="4" t="n">
+        <v>0.3405566</v>
+      </c>
+      <c r="D177" s="4" t="n">
+        <v>0.4146598</v>
+      </c>
+      <c r="E177" s="4" t="n">
+        <v>0.41823</v>
+      </c>
+      <c r="F177" s="4" t="n">
+        <v>1.040247</v>
+      </c>
+      <c r="G177" s="4" t="n">
+        <v>0.4970366</v>
+      </c>
+      <c r="H177" s="4"/>
+      <c r="I177" s="4"/>
+    </row>
+    <row r="178" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A178" s="4" t="s">
+        <v>222</v>
+      </c>
+      <c r="B178" s="4" t="s">
+        <v>223</v>
+      </c>
+      <c r="C178" s="4" t="n">
+        <v>0.3949252</v>
+      </c>
+      <c r="D178" s="4" t="n">
+        <v>0.3823582</v>
+      </c>
+      <c r="E178" s="4" t="n">
+        <v>0.4447452</v>
+      </c>
+      <c r="F178" s="4" t="n">
+        <v>1.2471894</v>
+      </c>
+      <c r="G178" s="4" t="n">
+        <v>0.4368736</v>
+      </c>
+      <c r="H178" s="4"/>
+      <c r="I178" s="4"/>
+    </row>
+    <row r="179" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A179" s="4" t="s">
+        <v>222</v>
+      </c>
+      <c r="B179" s="4" t="s">
+        <v>224</v>
+      </c>
+      <c r="C179" s="4" t="n">
+        <v>0.4043766</v>
+      </c>
+      <c r="D179" s="4" t="n">
+        <v>0.4442056</v>
+      </c>
+      <c r="E179" s="4" t="n">
+        <v>0.4380336</v>
+      </c>
+      <c r="F179" s="4" t="n">
+        <v>1.0671104</v>
+      </c>
+      <c r="G179" s="4" t="n">
+        <v>0.4808172</v>
+      </c>
+      <c r="H179" s="4"/>
+      <c r="I179" s="4"/>
+    </row>
+    <row r="180" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A180" s="4" t="s">
+        <v>222</v>
+      </c>
+      <c r="B180" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="C180" s="4" t="n">
+        <v>0.3432752</v>
+      </c>
+      <c r="D180" s="4" t="n">
+        <v>0.4025714</v>
+      </c>
+      <c r="E180" s="4" t="n">
+        <v>0.4243366</v>
+      </c>
+      <c r="F180" s="4" t="n">
+        <v>1.1215862</v>
+      </c>
+      <c r="G180" s="4" t="n">
+        <v>0.4852742</v>
+      </c>
+      <c r="H180" s="4"/>
+      <c r="I180" s="4"/>
     </row>
     <row r="1048567" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="1048568" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -13888,8 +14938,8 @@
   </sheetPr>
   <dimension ref="A1:AMJ1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A162" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D165" activeCellId="0" sqref="D165"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A168" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D180" activeCellId="0" sqref="D180"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -13935,7 +14985,7 @@
         <v>11</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>302</v>
+        <v>325</v>
       </c>
       <c r="C2" s="4" t="n">
         <v>3.4656902</v>
@@ -13958,7 +15008,7 @@
         <v>11</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>253</v>
+        <v>275</v>
       </c>
       <c r="C3" s="4" t="n">
         <v>4.0852622</v>
@@ -13981,7 +15031,7 @@
         <v>11</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>254</v>
+        <v>276</v>
       </c>
       <c r="C4" s="4" t="n">
         <v>2.9817282</v>
@@ -14004,7 +15054,7 @@
         <v>15</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>255</v>
+        <v>277</v>
       </c>
       <c r="C5" s="4" t="n">
         <v>3.2355116</v>
@@ -14073,7 +15123,7 @@
         <v>19</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>213</v>
+        <v>229</v>
       </c>
       <c r="C8" s="4" t="n">
         <v>3.7434734</v>
@@ -14096,7 +15146,7 @@
         <v>19</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>257</v>
+        <v>279</v>
       </c>
       <c r="C9" s="4" t="n">
         <v>3.5561424</v>
@@ -14119,7 +15169,7 @@
         <v>19</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>303</v>
+        <v>326</v>
       </c>
       <c r="C10" s="4" t="n">
         <v>3.2355472</v>
@@ -14142,7 +15192,7 @@
         <v>23</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>290</v>
+        <v>311</v>
       </c>
       <c r="C11" s="4" t="n">
         <v>3.8741284</v>
@@ -14165,7 +15215,7 @@
         <v>23</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>292</v>
+        <v>313</v>
       </c>
       <c r="C12" s="4" t="n">
         <v>3.5923944</v>
@@ -14234,7 +15284,7 @@
         <v>27</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>217</v>
+        <v>233</v>
       </c>
       <c r="C15" s="4" t="n">
         <v>3.0850886</v>
@@ -14257,7 +15307,7 @@
         <v>27</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>257</v>
+        <v>279</v>
       </c>
       <c r="C16" s="4" t="n">
         <v>4.2818632</v>
@@ -14303,7 +15353,7 @@
         <v>31</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>258</v>
+        <v>216</v>
       </c>
       <c r="C18" s="4" t="n">
         <v>3.5907182</v>
@@ -14326,7 +15376,7 @@
         <v>31</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>259</v>
+        <v>280</v>
       </c>
       <c r="C19" s="4" t="n">
         <v>2.8087598</v>
@@ -14349,7 +15399,7 @@
         <v>35</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>304</v>
+        <v>327</v>
       </c>
       <c r="C20" s="4" t="n">
         <v>3.0989676</v>
@@ -14372,7 +15422,7 @@
         <v>35</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>305</v>
+        <v>268</v>
       </c>
       <c r="C21" s="4" t="n">
         <v>2.9089418</v>
@@ -14441,7 +15491,7 @@
         <v>39</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>261</v>
+        <v>282</v>
       </c>
       <c r="C24" s="4" t="n">
         <v>3.6907394</v>
@@ -14487,7 +15537,7 @@
         <v>39</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>306</v>
+        <v>328</v>
       </c>
       <c r="C26" s="4" t="n">
         <v>3.822524</v>
@@ -14510,7 +15560,7 @@
         <v>39</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>307</v>
+        <v>329</v>
       </c>
       <c r="C27" s="4" t="n">
         <v>3.2866498</v>
@@ -14533,7 +15583,7 @@
         <v>39</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>308</v>
+        <v>330</v>
       </c>
       <c r="C28" s="4" t="n">
         <v>3.8178666</v>
@@ -14579,7 +15629,7 @@
         <v>46</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>309</v>
+        <v>331</v>
       </c>
       <c r="C30" s="4" t="n">
         <v>3.0702744</v>
@@ -14648,7 +15698,7 @@
         <v>50</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>310</v>
+        <v>332</v>
       </c>
       <c r="C33" s="4" t="n">
         <v>3.6235082</v>
@@ -14671,7 +15721,7 @@
         <v>50</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>311</v>
+        <v>333</v>
       </c>
       <c r="C34" s="4" t="n">
         <v>2.9263998</v>
@@ -14717,7 +15767,7 @@
         <v>53</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>255</v>
+        <v>277</v>
       </c>
       <c r="C36" s="4" t="n">
         <v>3.2355116</v>
@@ -14763,7 +15813,7 @@
         <v>56</v>
       </c>
       <c r="B38" s="4" t="s">
-        <v>312</v>
+        <v>334</v>
       </c>
       <c r="C38" s="4" t="n">
         <v>4.4183598</v>
@@ -14786,7 +15836,7 @@
         <v>56</v>
       </c>
       <c r="B39" s="4" t="s">
-        <v>313</v>
+        <v>335</v>
       </c>
       <c r="C39" s="4" t="n">
         <v>4.2271066</v>
@@ -14809,7 +15859,7 @@
         <v>56</v>
       </c>
       <c r="B40" s="4" t="s">
-        <v>314</v>
+        <v>336</v>
       </c>
       <c r="C40" s="4" t="n">
         <v>4.3486802</v>
@@ -14855,7 +15905,7 @@
         <v>60</v>
       </c>
       <c r="B42" s="4" t="s">
-        <v>212</v>
+        <v>228</v>
       </c>
       <c r="C42" s="4" t="n">
         <v>3.6324914</v>
@@ -14901,7 +15951,7 @@
         <v>64</v>
       </c>
       <c r="B44" s="4" t="s">
-        <v>315</v>
+        <v>337</v>
       </c>
       <c r="C44" s="4" t="n">
         <v>3.8775138</v>
@@ -14947,7 +15997,7 @@
         <v>64</v>
       </c>
       <c r="B46" s="4" t="s">
-        <v>274</v>
+        <v>295</v>
       </c>
       <c r="C46" s="4" t="n">
         <v>3.8538836</v>
@@ -15062,7 +16112,7 @@
         <v>72</v>
       </c>
       <c r="B51" s="4" t="s">
-        <v>275</v>
+        <v>296</v>
       </c>
       <c r="C51" s="4" t="n">
         <v>4.7661336</v>
@@ -15085,7 +16135,7 @@
         <v>72</v>
       </c>
       <c r="B52" s="4" t="s">
-        <v>316</v>
+        <v>338</v>
       </c>
       <c r="C52" s="4" t="n">
         <v>4.1553188</v>
@@ -15108,7 +16158,7 @@
         <v>76</v>
       </c>
       <c r="B53" s="4" t="s">
-        <v>276</v>
+        <v>297</v>
       </c>
       <c r="C53" s="4" t="n">
         <v>4.4161086</v>
@@ -15131,7 +16181,7 @@
         <v>76</v>
       </c>
       <c r="B54" s="4" t="s">
-        <v>317</v>
+        <v>339</v>
       </c>
       <c r="C54" s="4" t="n">
         <v>3.9109934</v>
@@ -15154,7 +16204,7 @@
         <v>76</v>
       </c>
       <c r="B55" s="4" t="s">
-        <v>310</v>
+        <v>332</v>
       </c>
       <c r="C55" s="4" t="n">
         <v>3.9109934</v>
@@ -15177,7 +16227,7 @@
         <v>80</v>
       </c>
       <c r="B56" s="4" t="s">
-        <v>277</v>
+        <v>298</v>
       </c>
       <c r="C56" s="4" t="n">
         <v>3.4861618</v>
@@ -15223,7 +16273,7 @@
         <v>80</v>
       </c>
       <c r="B58" s="4" t="s">
-        <v>318</v>
+        <v>340</v>
       </c>
       <c r="C58" s="4" t="n">
         <v>3.52287</v>
@@ -15407,7 +16457,7 @@
         <v>91</v>
       </c>
       <c r="B66" s="4" t="s">
-        <v>233</v>
+        <v>249</v>
       </c>
       <c r="C66" s="4" t="n">
         <v>4.0686228</v>
@@ -15430,7 +16480,7 @@
         <v>91</v>
       </c>
       <c r="B67" s="4" t="s">
-        <v>281</v>
+        <v>302</v>
       </c>
       <c r="C67" s="4" t="n">
         <v>3.0381616</v>
@@ -15453,7 +16503,7 @@
         <v>95</v>
       </c>
       <c r="B68" s="4" t="s">
-        <v>282</v>
+        <v>303</v>
       </c>
       <c r="C68" s="4" t="n">
         <v>3.9888114</v>
@@ -15476,7 +16526,7 @@
         <v>95</v>
       </c>
       <c r="B69" s="4" t="s">
-        <v>283</v>
+        <v>304</v>
       </c>
       <c r="C69" s="4" t="n">
         <v>4.1137066</v>
@@ -15499,7 +16549,7 @@
         <v>95</v>
       </c>
       <c r="B70" s="4" t="s">
-        <v>319</v>
+        <v>341</v>
       </c>
       <c r="C70" s="4" t="n">
         <v>4.983335</v>
@@ -15637,7 +16687,7 @@
         <v>103</v>
       </c>
       <c r="B76" s="4" t="s">
-        <v>320</v>
+        <v>342</v>
       </c>
       <c r="C76" s="4" t="n">
         <v>4.5492628</v>
@@ -15706,7 +16756,7 @@
         <v>107</v>
       </c>
       <c r="B79" s="4" t="s">
-        <v>238</v>
+        <v>254</v>
       </c>
       <c r="C79" s="4" t="n">
         <v>4.5622134</v>
@@ -16028,7 +17078,7 @@
         <v>126</v>
       </c>
       <c r="B93" s="4" t="s">
-        <v>240</v>
+        <v>256</v>
       </c>
       <c r="C93" s="4" t="n">
         <v>4.559301</v>
@@ -16120,7 +17170,7 @@
         <v>127</v>
       </c>
       <c r="B97" s="4" t="s">
-        <v>288</v>
+        <v>309</v>
       </c>
       <c r="C97" s="4" t="n">
         <v>3.7013772</v>
@@ -16189,7 +17239,7 @@
         <v>131</v>
       </c>
       <c r="B100" s="4" t="s">
-        <v>278</v>
+        <v>299</v>
       </c>
       <c r="C100" s="4" t="n">
         <v>4.1470936</v>
@@ -16212,7 +17262,7 @@
         <v>134</v>
       </c>
       <c r="B101" s="4" t="s">
-        <v>289</v>
+        <v>310</v>
       </c>
       <c r="C101" s="4" t="n">
         <v>4.5941812</v>
@@ -16258,7 +17308,7 @@
         <v>134</v>
       </c>
       <c r="B103" s="4" t="s">
-        <v>321</v>
+        <v>343</v>
       </c>
       <c r="C103" s="4" t="n">
         <v>4.2355866</v>
@@ -16350,7 +17400,7 @@
         <v>139</v>
       </c>
       <c r="B107" s="4" t="s">
-        <v>290</v>
+        <v>311</v>
       </c>
       <c r="C107" s="4" t="n">
         <v>3.9397008</v>
@@ -16373,7 +17423,7 @@
         <v>139</v>
       </c>
       <c r="B108" s="4" t="s">
-        <v>291</v>
+        <v>312</v>
       </c>
       <c r="C108" s="4" t="n">
         <v>3.8446282</v>
@@ -16396,7 +17446,7 @@
         <v>139</v>
       </c>
       <c r="B109" s="4" t="s">
-        <v>292</v>
+        <v>313</v>
       </c>
       <c r="C109" s="4" t="n">
         <v>3.6811188</v>
@@ -16419,7 +17469,7 @@
         <v>142</v>
       </c>
       <c r="B110" s="4" t="s">
-        <v>293</v>
+        <v>314</v>
       </c>
       <c r="C110" s="4" t="n">
         <v>4.0021732</v>
@@ -16580,7 +17630,7 @@
         <v>148</v>
       </c>
       <c r="B117" s="4" t="s">
-        <v>294</v>
+        <v>315</v>
       </c>
       <c r="C117" s="4" t="n">
         <v>3.9349018</v>
@@ -16672,7 +17722,7 @@
         <v>152</v>
       </c>
       <c r="B121" s="4" t="s">
-        <v>322</v>
+        <v>344</v>
       </c>
       <c r="C121" s="4" t="n">
         <v>3.7466574</v>
@@ -16741,7 +17791,7 @@
         <v>156</v>
       </c>
       <c r="B124" s="4" t="s">
-        <v>323</v>
+        <v>345</v>
       </c>
       <c r="C124" s="4" t="n">
         <v>3.986907</v>
@@ -16787,7 +17837,7 @@
         <v>160</v>
       </c>
       <c r="B126" s="4" t="s">
-        <v>267</v>
+        <v>288</v>
       </c>
       <c r="C126" s="4" t="n">
         <v>3.6994948</v>
@@ -16879,7 +17929,7 @@
         <v>164</v>
       </c>
       <c r="B130" s="4" t="s">
-        <v>324</v>
+        <v>346</v>
       </c>
       <c r="C130" s="4" t="n">
         <v>4.1747286</v>
@@ -16902,7 +17952,7 @@
         <v>167</v>
       </c>
       <c r="B131" s="4" t="s">
-        <v>325</v>
+        <v>347</v>
       </c>
       <c r="C131" s="4" t="n">
         <v>3.529065</v>
@@ -17040,7 +18090,7 @@
         <v>169</v>
       </c>
       <c r="B137" s="4" t="s">
-        <v>280</v>
+        <v>301</v>
       </c>
       <c r="C137" s="4" t="n">
         <v>3.1387814</v>
@@ -17178,7 +18228,7 @@
         <v>182</v>
       </c>
       <c r="B143" s="4" t="s">
-        <v>255</v>
+        <v>277</v>
       </c>
       <c r="C143" s="4" t="n">
         <v>3.6613182</v>
@@ -17278,7 +18328,7 @@
         <v>184</v>
       </c>
       <c r="B147" s="4" t="s">
-        <v>326</v>
+        <v>348</v>
       </c>
       <c r="C147" s="4" t="n">
         <v>4.9899384</v>
@@ -17303,7 +18353,7 @@
         <v>184</v>
       </c>
       <c r="B148" s="4" t="s">
-        <v>297</v>
+        <v>318</v>
       </c>
       <c r="C148" s="4" t="n">
         <v>4.6078064</v>
@@ -17428,7 +18478,7 @@
         <v>189</v>
       </c>
       <c r="B153" s="4" t="s">
-        <v>327</v>
+        <v>349</v>
       </c>
       <c r="C153" s="4" t="n">
         <v>3.3410662</v>
@@ -17503,7 +18553,7 @@
         <v>192</v>
       </c>
       <c r="B156" s="4" t="s">
-        <v>328</v>
+        <v>350</v>
       </c>
       <c r="C156" s="4" t="n">
         <v>3.6757588</v>
@@ -17578,7 +18628,7 @@
         <v>196</v>
       </c>
       <c r="B159" s="4" t="s">
-        <v>300</v>
+        <v>321</v>
       </c>
       <c r="C159" s="4" t="n">
         <v>3.1456856</v>
@@ -17648,7 +18698,7 @@
       <c r="H161" s="4"/>
       <c r="I161" s="4"/>
     </row>
-    <row r="162" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="162" customFormat="false" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A162" s="4" t="s">
         <v>200</v>
       </c>
@@ -17673,12 +18723,12 @@
       <c r="H162" s="4"/>
       <c r="I162" s="4"/>
     </row>
-    <row r="163" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="163" customFormat="false" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A163" s="4" t="s">
         <v>203</v>
       </c>
       <c r="B163" s="4" t="s">
-        <v>329</v>
+        <v>351</v>
       </c>
       <c r="C163" s="4" t="n">
         <v>3.365378</v>
@@ -17698,7 +18748,7 @@
       <c r="H163" s="4"/>
       <c r="I163" s="4"/>
     </row>
-    <row r="164" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="164" customFormat="false" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A164" s="4" t="s">
         <v>203</v>
       </c>
@@ -17723,7 +18773,7 @@
       <c r="H164" s="4"/>
       <c r="I164" s="4"/>
     </row>
-    <row r="165" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="165" customFormat="false" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A165" s="4" t="s">
         <v>203</v>
       </c>
@@ -17748,7 +18798,7 @@
       <c r="H165" s="4"/>
       <c r="I165" s="4"/>
     </row>
-    <row r="166" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="166" customFormat="false" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A166" s="4" t="s">
         <v>207</v>
       </c>
@@ -17773,12 +18823,12 @@
       <c r="H166" s="4"/>
       <c r="I166" s="4"/>
     </row>
-    <row r="167" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="167" customFormat="false" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A167" s="4" t="s">
         <v>207</v>
       </c>
       <c r="B167" s="4" t="s">
-        <v>301</v>
+        <v>322</v>
       </c>
       <c r="C167" s="4" t="n">
         <v>3.7039678</v>
@@ -17798,12 +18848,12 @@
       <c r="H167" s="4"/>
       <c r="I167" s="4"/>
     </row>
-    <row r="168" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="168" customFormat="false" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A168" s="4" t="s">
         <v>207</v>
       </c>
       <c r="B168" s="4" t="s">
-        <v>330</v>
+        <v>352</v>
       </c>
       <c r="C168" s="4" t="n">
         <v>3.7096014</v>
@@ -17822,6 +18872,331 @@
       </c>
       <c r="H168" s="4"/>
       <c r="I168" s="4"/>
+    </row>
+    <row r="169" customFormat="false" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A169" s="4" t="s">
+        <v>211</v>
+      </c>
+      <c r="B169" s="4" t="s">
+        <v>353</v>
+      </c>
+      <c r="C169" s="4" t="n">
+        <v>5.4967574</v>
+      </c>
+      <c r="D169" s="4" t="n">
+        <v>2.9669744</v>
+      </c>
+      <c r="E169" s="4" t="n">
+        <v>1.613153</v>
+      </c>
+      <c r="F169" s="4" t="n">
+        <v>2.3278236</v>
+      </c>
+      <c r="G169" s="4" t="n">
+        <v>1.1525834</v>
+      </c>
+      <c r="H169" s="4"/>
+      <c r="I169" s="4"/>
+    </row>
+    <row r="170" customFormat="false" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A170" s="4" t="s">
+        <v>211</v>
+      </c>
+      <c r="B170" s="4" t="s">
+        <v>213</v>
+      </c>
+      <c r="C170" s="4" t="n">
+        <v>3.777915</v>
+      </c>
+      <c r="D170" s="4" t="n">
+        <v>1.6785774</v>
+      </c>
+      <c r="E170" s="4" t="n">
+        <v>1.4178596</v>
+      </c>
+      <c r="F170" s="4" t="n">
+        <v>2.8642304</v>
+      </c>
+      <c r="G170" s="4" t="n">
+        <v>1.41006</v>
+      </c>
+      <c r="H170" s="4"/>
+      <c r="I170" s="4"/>
+    </row>
+    <row r="171" customFormat="false" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A171" s="4" t="s">
+        <v>211</v>
+      </c>
+      <c r="B171" s="4" t="s">
+        <v>259</v>
+      </c>
+      <c r="C171" s="4" t="n">
+        <v>4.669323</v>
+      </c>
+      <c r="D171" s="4" t="n">
+        <v>2.6768006</v>
+      </c>
+      <c r="E171" s="4" t="n">
+        <v>1.8010994</v>
+      </c>
+      <c r="F171" s="4" t="n">
+        <v>2.588558</v>
+      </c>
+      <c r="G171" s="4" t="n">
+        <v>1.5023306</v>
+      </c>
+      <c r="H171" s="4"/>
+      <c r="I171" s="4"/>
+    </row>
+    <row r="172" customFormat="false" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A172" s="4" t="s">
+        <v>215</v>
+      </c>
+      <c r="B172" s="4" t="s">
+        <v>216</v>
+      </c>
+      <c r="C172" s="4" t="n">
+        <v>3.3072694</v>
+      </c>
+      <c r="D172" s="4" t="n">
+        <v>1.9006078</v>
+      </c>
+      <c r="E172" s="4" t="n">
+        <v>1.1850164</v>
+      </c>
+      <c r="F172" s="4" t="n">
+        <v>2.6602388</v>
+      </c>
+      <c r="G172" s="4" t="n">
+        <v>0.9476772</v>
+      </c>
+      <c r="H172" s="4"/>
+      <c r="I172" s="4"/>
+    </row>
+    <row r="173" customFormat="false" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A173" s="4" t="s">
+        <v>215</v>
+      </c>
+      <c r="B173" s="4" t="s">
+        <v>217</v>
+      </c>
+      <c r="C173" s="4" t="n">
+        <v>2.8846846</v>
+      </c>
+      <c r="D173" s="4" t="n">
+        <v>1.3024432</v>
+      </c>
+      <c r="E173" s="4" t="n">
+        <v>1.2235786</v>
+      </c>
+      <c r="F173" s="4" t="n">
+        <v>2.0758566</v>
+      </c>
+      <c r="G173" s="4" t="n">
+        <v>1.044621</v>
+      </c>
+      <c r="H173" s="4"/>
+      <c r="I173" s="4"/>
+    </row>
+    <row r="174" customFormat="false" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A174" s="4" t="s">
+        <v>215</v>
+      </c>
+      <c r="B174" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C174" s="4" t="n">
+        <v>3.1142618</v>
+      </c>
+      <c r="D174" s="4" t="n">
+        <v>1.0677274</v>
+      </c>
+      <c r="E174" s="4" t="n">
+        <v>0.87897</v>
+      </c>
+      <c r="F174" s="4" t="n">
+        <v>2.1044836</v>
+      </c>
+      <c r="G174" s="4" t="n">
+        <v>1.0777108</v>
+      </c>
+      <c r="H174" s="4"/>
+      <c r="I174" s="4"/>
+    </row>
+    <row r="175" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A175" s="4" t="s">
+        <v>215</v>
+      </c>
+      <c r="B175" s="4" t="s">
+        <v>219</v>
+      </c>
+      <c r="C175" s="4" t="n">
+        <v>4.0107472</v>
+      </c>
+      <c r="D175" s="4" t="n">
+        <v>1.2319864</v>
+      </c>
+      <c r="E175" s="4" t="n">
+        <v>1.3148566</v>
+      </c>
+      <c r="F175" s="4" t="n">
+        <v>2.3331034</v>
+      </c>
+      <c r="G175" s="4" t="n">
+        <v>0.9706266</v>
+      </c>
+      <c r="H175" s="4"/>
+      <c r="I175" s="4"/>
+    </row>
+    <row r="176" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A176" s="4" t="s">
+        <v>215</v>
+      </c>
+      <c r="B176" s="4" t="s">
+        <v>221</v>
+      </c>
+      <c r="C176" s="4" t="n">
+        <v>3.5906696</v>
+      </c>
+      <c r="D176" s="4" t="n">
+        <v>1.1616654</v>
+      </c>
+      <c r="E176" s="4" t="n">
+        <v>0.8514104</v>
+      </c>
+      <c r="F176" s="4" t="n">
+        <v>2.3141506</v>
+      </c>
+      <c r="G176" s="4" t="n">
+        <v>1.0083712</v>
+      </c>
+      <c r="H176" s="4"/>
+      <c r="I176" s="4"/>
+    </row>
+    <row r="177" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A177" s="4" t="s">
+        <v>215</v>
+      </c>
+      <c r="B177" s="4" t="s">
+        <v>354</v>
+      </c>
+      <c r="C177" s="4" t="n">
+        <v>3.6453918</v>
+      </c>
+      <c r="D177" s="4" t="n">
+        <v>1.0535136</v>
+      </c>
+      <c r="E177" s="4" t="n">
+        <v>1.2287252</v>
+      </c>
+      <c r="F177" s="4" t="n">
+        <v>2.3464962</v>
+      </c>
+      <c r="G177" s="4" t="n">
+        <v>0.9529058</v>
+      </c>
+      <c r="H177" s="4"/>
+      <c r="I177" s="4"/>
+    </row>
+    <row r="178" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A178" s="4" t="s">
+        <v>215</v>
+      </c>
+      <c r="B178" s="4" t="s">
+        <v>272</v>
+      </c>
+      <c r="C178" s="4" t="n">
+        <v>3.0646552</v>
+      </c>
+      <c r="D178" s="4" t="n">
+        <v>1.3052728</v>
+      </c>
+      <c r="E178" s="4" t="n">
+        <v>1.208871</v>
+      </c>
+      <c r="F178" s="4" t="n">
+        <v>2.1763898</v>
+      </c>
+      <c r="G178" s="4" t="n">
+        <v>1.0785698</v>
+      </c>
+      <c r="H178" s="4"/>
+      <c r="I178" s="4"/>
+    </row>
+    <row r="179" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A179" s="4" t="s">
+        <v>222</v>
+      </c>
+      <c r="B179" s="4" t="s">
+        <v>223</v>
+      </c>
+      <c r="C179" s="4" t="n">
+        <v>3.828837</v>
+      </c>
+      <c r="D179" s="4" t="n">
+        <v>2.250791</v>
+      </c>
+      <c r="E179" s="4" t="n">
+        <v>1.0752212</v>
+      </c>
+      <c r="F179" s="4" t="n">
+        <v>2.5408678</v>
+      </c>
+      <c r="G179" s="4" t="n">
+        <v>1.0408466</v>
+      </c>
+      <c r="H179" s="4"/>
+      <c r="I179" s="4"/>
+    </row>
+    <row r="180" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A180" s="4" t="s">
+        <v>222</v>
+      </c>
+      <c r="B180" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="C180" s="4" t="n">
+        <v>3.6186178</v>
+      </c>
+      <c r="D180" s="4" t="n">
+        <v>1.1495222</v>
+      </c>
+      <c r="E180" s="4" t="n">
+        <v>0.7760448</v>
+      </c>
+      <c r="F180" s="4" t="n">
+        <v>2.1896554</v>
+      </c>
+      <c r="G180" s="4" t="n">
+        <v>0.9280454</v>
+      </c>
+      <c r="H180" s="4"/>
+      <c r="I180" s="4"/>
+    </row>
+    <row r="181" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A181" s="4" t="s">
+        <v>222</v>
+      </c>
+      <c r="B181" s="4" t="s">
+        <v>355</v>
+      </c>
+      <c r="C181" s="4" t="n">
+        <v>3.3664146</v>
+      </c>
+      <c r="D181" s="4" t="n">
+        <v>1.2025386</v>
+      </c>
+      <c r="E181" s="4" t="n">
+        <v>0.825262</v>
+      </c>
+      <c r="F181" s="4" t="n">
+        <v>2.1805336</v>
+      </c>
+      <c r="G181" s="4" t="n">
+        <v>1.0091106</v>
+      </c>
+      <c r="H181" s="4"/>
+      <c r="I181" s="4"/>
     </row>
     <row r="1048567" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="1048568" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>

</xml_diff>